<commit_message>
Added MC1 & MC1.1
I've added MC1 and MC1.1 as two similar but distinct collars, along with their own documentation.
MC1.1 is still WIP at the moment.
</commit_message>
<xml_diff>
--- a/Medium Collar/MC1.1 Mk1 PBS.xlsx
+++ b/Medium Collar/MC1.1 Mk1 PBS.xlsx
@@ -1,23 +1,29 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24701"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Storage\Documents\Work files\Ishaan - Conservation Data Collection\MediumCollar1\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Storage\Documents\GitHub\Trak-TFRC-System\Medium Collar\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EFEABEE7-038F-4071-AB1D-C64B69B356AF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F84CE32-8077-4941-9485-C7E8AD3ED817}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="PBS" sheetId="1" r:id="rId1"/>
-    <sheet name="PCB Assembly Ref" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
     <ext uri="GoogleSheetsCustomDataVersion1">
       <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId6" roundtripDataSignature="AMtx7mia0vo8kToBZ+bn4GNfUYeDdeZQvg=="/>
     </ext>
@@ -26,10 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="226" uniqueCount="178">
-  <si>
-    <t>MediumCollar1 - Product Breakdown Sheet</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="109">
   <si>
     <t>Pricing</t>
   </si>
@@ -98,9 +101,6 @@
   </si>
   <si>
     <t>MC1A00-000</t>
-  </si>
-  <si>
-    <t>MediumCollar1 Mk1</t>
   </si>
   <si>
     <t>CAD Completed</t>
@@ -439,211 +439,10 @@
     <t>Vacuum Formed</t>
   </si>
   <si>
-    <t>ECAD Version- v26</t>
-  </si>
-  <si>
-    <t>Qty</t>
-  </si>
-  <si>
-    <t>Value</t>
-  </si>
-  <si>
-    <t>Parts</t>
-  </si>
-  <si>
-    <t>Description</t>
-  </si>
-  <si>
-    <t>BACKUP_BATT1</t>
-  </si>
-  <si>
-    <t>Battery - Single Cell</t>
-  </si>
-  <si>
-    <t>SMA</t>
-  </si>
-  <si>
-    <t>SMA Connector</t>
-  </si>
-  <si>
-    <t>0.1uF</t>
-  </si>
-  <si>
-    <t>C3, C4, C5, C7, C14</t>
-  </si>
-  <si>
-    <t>Capacitor - Generic</t>
-  </si>
-  <si>
-    <t>0.96_OLED_I2C</t>
-  </si>
-  <si>
-    <t>OLED1</t>
-  </si>
-  <si>
-    <t>100uF</t>
-  </si>
-  <si>
-    <t>C10</t>
-  </si>
-  <si>
-    <t>Capacitor Polarised - Generic</t>
-  </si>
-  <si>
-    <t>10k</t>
-  </si>
-  <si>
-    <t>R3, R4, R5, R6</t>
-  </si>
-  <si>
-    <t>Resistor Fixed - Generic</t>
-  </si>
-  <si>
-    <t>10uF</t>
-  </si>
-  <si>
-    <t>C8, C9</t>
-  </si>
-  <si>
-    <t>1N5820</t>
-  </si>
-  <si>
-    <t>D1</t>
-  </si>
-  <si>
-    <t>Schottky Diode - Popular parts</t>
-  </si>
-  <si>
-    <t>1P2T_SLIDE_SWITCH</t>
-  </si>
-  <si>
-    <t>S1</t>
-  </si>
-  <si>
-    <t>1uF</t>
-  </si>
-  <si>
-    <t>C11, C12, C13</t>
-  </si>
-  <si>
-    <t>33pF</t>
-  </si>
-  <si>
-    <t>C1, C2</t>
-  </si>
-  <si>
-    <t>4.7k</t>
-  </si>
-  <si>
-    <t>R1, R2</t>
-  </si>
-  <si>
-    <t>4.7uF</t>
-  </si>
-  <si>
-    <t>C6</t>
-  </si>
-  <si>
-    <t>470uF</t>
-  </si>
-  <si>
-    <t>C15</t>
-  </si>
-  <si>
-    <t>68uh</t>
-  </si>
-  <si>
-    <t>L1</t>
-  </si>
-  <si>
-    <t>8mhz</t>
-  </si>
-  <si>
-    <t>Q1</t>
-  </si>
-  <si>
-    <t>CRYSTAL</t>
-  </si>
-  <si>
-    <t>ATMEGA328P-AU</t>
-  </si>
-  <si>
-    <t>U1</t>
-  </si>
-  <si>
-    <t>8-bit AVR Microcontroller</t>
-  </si>
-  <si>
-    <t>DS3231MZ+</t>
-  </si>
-  <si>
-    <t>U5</t>
-  </si>
-  <si>
-    <t>PMOSFET</t>
-  </si>
-  <si>
-    <t>U3</t>
-  </si>
-  <si>
-    <t>LDO-LM11173.3MP</t>
-  </si>
-  <si>
-    <t>P2</t>
-  </si>
-  <si>
-    <t>800mA Low-Dropout Linear Regulator</t>
-  </si>
-  <si>
-    <t>LORA_RFM95W-915S2_MODULE</t>
-  </si>
-  <si>
-    <t>U4</t>
-  </si>
-  <si>
-    <t>MOMENTARY-SWITCH-SPST-PTH-12MM</t>
-  </si>
-  <si>
-    <t>S2, S3</t>
-  </si>
-  <si>
-    <t>Momentary Switch (Pushbutton) - SPST</t>
-  </si>
-  <si>
-    <t>MOMENTARY-SWITCH-SPST-PTH-6MM</t>
-  </si>
-  <si>
-    <t>S4</t>
-  </si>
-  <si>
-    <t>PA6H_GPS</t>
-  </si>
-  <si>
-    <t>U2</t>
-  </si>
-  <si>
-    <t>SD_MICRO_SOCKET-204270SD_FULL</t>
-  </si>
-  <si>
-    <t>SD</t>
-  </si>
-  <si>
-    <t>TERMINAL_BLOCK</t>
-  </si>
-  <si>
-    <t>JP3A, JP4A, JP5A</t>
-  </si>
-  <si>
-    <t>XL1509</t>
-  </si>
-  <si>
-    <t>P1</t>
-  </si>
-  <si>
-    <t>DC Power Jack</t>
-  </si>
-  <si>
-    <t>J1</t>
+    <t>MediumCollar1.1 - Product Breakdown Sheet</t>
+  </si>
+  <si>
+    <t>MediumCollar1.1 Mk1 (Electronic Release)</t>
   </si>
 </sst>
 </file>
@@ -653,7 +452,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="&quot;₹&quot;\ #,##0"/>
   </numFmts>
-  <fonts count="14" x14ac:knownFonts="1">
+  <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -712,18 +511,6 @@
       <sz val="11"/>
       <color rgb="FF0563C1"/>
       <name val="Arial"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
     </font>
     <font>
       <sz val="10"/>
@@ -837,7 +624,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="39">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="164" fontId="1" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -873,13 +660,6 @@
     <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -889,8 +669,6 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1109,7 +887,7 @@
   <dimension ref="A1:P1000"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L4" sqref="L4"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1134,81 +912,81 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A1" s="32" t="s">
+      <c r="A1" s="27" t="s">
+        <v>107</v>
+      </c>
+      <c r="B1" s="28"/>
+      <c r="C1" s="28"/>
+      <c r="D1" s="28"/>
+      <c r="E1" s="28"/>
+      <c r="F1" s="28"/>
+      <c r="G1" s="28"/>
+      <c r="H1" s="28"/>
+      <c r="I1" s="28"/>
+      <c r="J1" s="28"/>
+      <c r="K1" s="29" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="33"/>
-      <c r="C1" s="33"/>
-      <c r="D1" s="33"/>
-      <c r="E1" s="33"/>
-      <c r="F1" s="33"/>
-      <c r="G1" s="33"/>
-      <c r="H1" s="33"/>
-      <c r="I1" s="33"/>
-      <c r="J1" s="33"/>
-      <c r="K1" s="34" t="s">
+      <c r="L1" s="28"/>
+      <c r="M1" s="1"/>
+      <c r="O1" s="30" t="s">
         <v>1</v>
       </c>
-      <c r="L1" s="33"/>
-      <c r="M1" s="1"/>
-      <c r="O1" s="35" t="s">
-        <v>2</v>
-      </c>
-      <c r="P1" s="36"/>
+      <c r="P1" s="31"/>
     </row>
     <row r="2" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="C2" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="D2" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="E2" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="F2" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="F2" s="2" t="s">
+      <c r="G2" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="G2" s="3" t="s">
+      <c r="H2" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="H2" s="4" t="s">
+      <c r="I2" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="I2" s="2" t="s">
+      <c r="J2" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="J2" s="2" t="s">
+      <c r="K2" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="K2" s="5" t="s">
+      <c r="L2" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="L2" s="5" t="s">
+      <c r="M2" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="M2" s="5" t="s">
+      <c r="O2" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="O2" s="6" t="s">
+      <c r="P2" s="7" t="s">
         <v>16</v>
-      </c>
-      <c r="P2" s="7" t="s">
-        <v>17</v>
       </c>
     </row>
     <row r="3" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="8" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B3" s="9" t="s">
-        <v>19</v>
+        <v>108</v>
       </c>
       <c r="C3" s="10"/>
       <c r="D3" s="10"/>
@@ -1221,7 +999,7 @@
         <v>40</v>
       </c>
       <c r="I3" s="8" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="J3" s="10"/>
       <c r="K3" s="13"/>
@@ -1235,15 +1013,15 @@
       </c>
       <c r="O3" s="14"/>
       <c r="P3" s="7" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
     </row>
     <row r="4" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="8" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B4" s="15" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C4" s="10"/>
       <c r="D4" s="10"/>
@@ -1252,7 +1030,7 @@
       <c r="G4" s="11"/>
       <c r="H4" s="12"/>
       <c r="I4" s="8" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="J4" s="10"/>
       <c r="K4" s="13"/>
@@ -1260,30 +1038,30 @@
       <c r="M4" s="13"/>
       <c r="O4" s="14"/>
       <c r="P4" s="7" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A5" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="B5" s="16" t="s">
+        <v>24</v>
+      </c>
+      <c r="C5" s="17" t="s">
         <v>25</v>
       </c>
-      <c r="B5" s="16" t="s">
+      <c r="E5" s="10" t="s">
         <v>26</v>
-      </c>
-      <c r="C5" s="17" t="s">
-        <v>27</v>
-      </c>
-      <c r="E5" s="10" t="s">
-        <v>28</v>
       </c>
       <c r="G5" s="17">
         <v>1</v>
       </c>
       <c r="I5" s="8" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="J5" s="16" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="K5" s="18">
         <v>360</v>
@@ -1295,24 +1073,24 @@
       <c r="M5" s="13"/>
       <c r="O5" s="14"/>
       <c r="P5" s="7" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="6" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A6" s="8" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B6" s="16" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C6" s="17" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="G6" s="16">
         <v>1</v>
       </c>
       <c r="I6" s="8" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="K6" s="19">
         <v>80</v>
@@ -1323,58 +1101,58 @@
       </c>
       <c r="M6" s="13"/>
       <c r="O6" s="14" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="P6" s="14" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="7" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A7" s="8" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B7" s="16" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C7" s="17" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="G7" s="16">
         <v>1</v>
       </c>
       <c r="I7" s="8" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="L7" s="13">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="O7" s="14" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="P7" s="14"/>
     </row>
     <row r="8" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A8" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="B8" s="20" t="s">
+        <v>35</v>
+      </c>
+      <c r="C8" s="16" t="s">
         <v>36</v>
       </c>
-      <c r="B8" s="20" t="s">
+      <c r="D8" s="16" t="s">
         <v>37</v>
       </c>
-      <c r="C8" s="16" t="s">
+      <c r="F8" s="16" t="s">
         <v>38</v>
-      </c>
-      <c r="D8" s="16" t="s">
-        <v>39</v>
-      </c>
-      <c r="F8" s="16" t="s">
-        <v>40</v>
       </c>
       <c r="G8" s="16">
         <v>1</v>
       </c>
       <c r="I8" s="8" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="K8" s="16">
         <v>475</v>
@@ -1384,33 +1162,33 @@
         <v>475</v>
       </c>
       <c r="O8" s="14" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="P8" s="21" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
     </row>
     <row r="9" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A9" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="B9" s="16" t="s">
+        <v>41</v>
+      </c>
+      <c r="C9" s="16" t="s">
+        <v>36</v>
+      </c>
+      <c r="D9" s="16" t="s">
         <v>42</v>
       </c>
-      <c r="B9" s="16" t="s">
+      <c r="F9" s="16" t="s">
         <v>43</v>
-      </c>
-      <c r="C9" s="16" t="s">
-        <v>38</v>
-      </c>
-      <c r="D9" s="16" t="s">
-        <v>44</v>
-      </c>
-      <c r="F9" s="16" t="s">
-        <v>45</v>
       </c>
       <c r="G9" s="16">
         <v>5</v>
       </c>
       <c r="I9" s="8" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="K9" s="16">
         <v>5.6</v>
@@ -1420,60 +1198,60 @@
         <v>28</v>
       </c>
       <c r="O9" s="14" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="P9" s="21" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
     </row>
     <row r="10" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A10" s="8" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="B10" s="16" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="C10" s="16" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="G10" s="16">
         <v>1</v>
       </c>
       <c r="I10" s="8" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="J10" s="16" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="L10" s="13">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="O10" s="14" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="P10" s="21" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
     </row>
     <row r="11" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A11" s="8" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B11" s="16" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C11" s="16" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="G11" s="16">
         <v>1</v>
       </c>
       <c r="I11" s="8" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="J11" s="16" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="K11" s="16">
         <v>212</v>
@@ -1483,30 +1261,30 @@
         <v>212</v>
       </c>
       <c r="O11" s="14" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="P11" s="14" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
     <row r="12" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A12" s="8" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B12" s="16" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="C12" s="17" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="G12" s="16">
         <v>1</v>
       </c>
       <c r="I12" s="8" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="J12" s="16" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="K12" s="16">
         <v>80</v>
@@ -1516,27 +1294,27 @@
         <v>80</v>
       </c>
       <c r="O12" s="14" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="P12" s="14" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
     </row>
     <row r="13" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A13" s="8" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="B13" s="16" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="C13" s="17" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="G13" s="16">
         <v>1</v>
       </c>
       <c r="I13" s="8" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="K13" s="16">
         <v>50</v>
@@ -1546,27 +1324,27 @@
         <v>50</v>
       </c>
       <c r="O13" s="14" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="P13" s="14" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
     </row>
     <row r="14" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A14" s="8" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="B14" s="16" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="C14" s="17" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="G14" s="16">
         <v>1</v>
       </c>
       <c r="I14" s="8" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="K14" s="20">
         <v>15</v>
@@ -1576,27 +1354,27 @@
         <v>15</v>
       </c>
       <c r="O14" s="14" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="P14" s="14" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
     </row>
     <row r="15" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A15" s="8" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="B15" s="16" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="C15" s="17" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="G15" s="16">
         <v>1</v>
       </c>
       <c r="I15" s="8" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="K15" s="20">
         <v>5</v>
@@ -1610,22 +1388,22 @@
     </row>
     <row r="16" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A16" s="8" t="s">
+        <v>69</v>
+      </c>
+      <c r="B16" s="16" t="s">
+        <v>70</v>
+      </c>
+      <c r="C16" s="16" t="s">
+        <v>36</v>
+      </c>
+      <c r="D16" s="16" t="s">
         <v>71</v>
-      </c>
-      <c r="B16" s="16" t="s">
-        <v>72</v>
-      </c>
-      <c r="C16" s="16" t="s">
-        <v>38</v>
-      </c>
-      <c r="D16" s="16" t="s">
-        <v>73</v>
       </c>
       <c r="G16" s="16">
         <v>1</v>
       </c>
       <c r="I16" s="8" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="K16" s="16">
         <v>9</v>
@@ -1635,30 +1413,30 @@
         <v>9</v>
       </c>
       <c r="O16" s="6" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="P16" s="14" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
     </row>
     <row r="17" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A17" s="8" t="s">
+        <v>74</v>
+      </c>
+      <c r="B17" s="16" t="s">
+        <v>75</v>
+      </c>
+      <c r="C17" s="16" t="s">
+        <v>36</v>
+      </c>
+      <c r="D17" s="20" t="s">
         <v>76</v>
-      </c>
-      <c r="B17" s="16" t="s">
-        <v>77</v>
-      </c>
-      <c r="C17" s="16" t="s">
-        <v>38</v>
-      </c>
-      <c r="D17" s="20" t="s">
-        <v>78</v>
       </c>
       <c r="G17" s="16">
         <v>1</v>
       </c>
       <c r="I17" s="8" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="L17" s="13">
         <f t="shared" si="0"/>
@@ -1666,30 +1444,30 @@
       </c>
       <c r="O17" s="14"/>
       <c r="P17" s="14" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
     </row>
     <row r="18" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A18" s="8" t="s">
+        <v>79</v>
+      </c>
+      <c r="B18" s="20" t="s">
+        <v>80</v>
+      </c>
+      <c r="C18" s="16" t="s">
+        <v>36</v>
+      </c>
+      <c r="D18" s="16" t="s">
         <v>81</v>
-      </c>
-      <c r="B18" s="20" t="s">
-        <v>82</v>
-      </c>
-      <c r="C18" s="16" t="s">
-        <v>38</v>
-      </c>
-      <c r="D18" s="16" t="s">
-        <v>83</v>
       </c>
       <c r="G18" s="20">
         <v>2</v>
       </c>
       <c r="I18" s="8" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="J18" s="16" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="K18" s="18">
         <v>3</v>
@@ -1701,54 +1479,54 @@
       <c r="M18" s="13"/>
       <c r="O18" s="14"/>
       <c r="P18" s="14" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
     </row>
     <row r="19" spans="1:16" ht="14.25" x14ac:dyDescent="0.2">
       <c r="O19" s="14"/>
       <c r="P19" s="14" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
     </row>
     <row r="20" spans="1:16" ht="14.25" x14ac:dyDescent="0.2">
       <c r="O20" s="14"/>
       <c r="P20" s="14" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
     </row>
     <row r="21" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B21" s="22" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="K21" s="23"/>
       <c r="L21" s="13"/>
       <c r="M21" s="13"/>
       <c r="O21" s="14"/>
       <c r="P21" s="14" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
     </row>
     <row r="22" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="8" t="s">
+        <v>86</v>
+      </c>
+      <c r="B22" s="24" t="s">
+        <v>87</v>
+      </c>
+      <c r="C22" s="17" t="s">
+        <v>36</v>
+      </c>
+      <c r="E22" s="10" t="s">
         <v>88</v>
       </c>
-      <c r="B22" s="24" t="s">
+      <c r="F22" s="25" t="s">
         <v>89</v>
-      </c>
-      <c r="C22" s="17" t="s">
-        <v>38</v>
-      </c>
-      <c r="E22" s="10" t="s">
-        <v>90</v>
-      </c>
-      <c r="F22" s="25" t="s">
-        <v>91</v>
       </c>
       <c r="G22" s="17">
         <v>0.05</v>
       </c>
       <c r="I22" s="10" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="K22" s="26">
         <v>320</v>
@@ -1760,7 +1538,7 @@
       <c r="M22" s="13"/>
       <c r="O22" s="14"/>
       <c r="P22" s="14" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="23" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1769,7 +1547,7 @@
       <c r="M23" s="13"/>
       <c r="O23" s="14"/>
       <c r="P23" s="14" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
     </row>
     <row r="24" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1778,12 +1556,12 @@
       <c r="M24" s="13"/>
       <c r="O24" s="14"/>
       <c r="P24" s="14" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
     </row>
     <row r="25" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B25" s="22" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="K25" s="13"/>
       <c r="L25" s="13"/>
@@ -1793,58 +1571,58 @@
     </row>
     <row r="26" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="O26" s="6" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="P26" s="14" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
     </row>
     <row r="27" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="O27" s="14"/>
       <c r="P27" s="14" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
     </row>
     <row r="28" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="O28" s="14"/>
       <c r="P28" s="14" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="29" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="O29" s="14"/>
       <c r="P29" s="14" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
     </row>
     <row r="30" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="O30" s="14"/>
       <c r="P30" s="14" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
     </row>
     <row r="31" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="O31" s="14"/>
       <c r="P31" s="14" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
     </row>
     <row r="32" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="O32" s="14"/>
       <c r="P32" s="14" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
     </row>
     <row r="33" spans="15:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="O33" s="14"/>
       <c r="P33" s="14" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
     </row>
     <row r="34" spans="15:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="O34" s="14"/>
       <c r="P34" s="14" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
     </row>
     <row r="35" spans="15:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -1857,52 +1635,52 @@
     </row>
     <row r="37" spans="15:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="O37" s="6" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="P37" s="14" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
     </row>
     <row r="38" spans="15:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="O38" s="14"/>
       <c r="P38" s="14" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
     </row>
     <row r="39" spans="15:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="O39" s="14"/>
       <c r="P39" s="14" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
     </row>
     <row r="40" spans="15:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="O40" s="14"/>
       <c r="P40" s="14" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
     </row>
     <row r="41" spans="15:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="O41" s="14"/>
       <c r="P41" s="14" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
     </row>
     <row r="42" spans="15:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="O42" s="14"/>
       <c r="P42" s="14" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
     </row>
     <row r="43" spans="15:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="O43" s="14"/>
       <c r="P43" s="14" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
     </row>
     <row r="44" spans="15:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="O44" s="14"/>
       <c r="P44" s="14" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
     </row>
     <row r="45" spans="15:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -2887,418 +2665,4 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup orientation="landscape"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <sheetPr>
-    <outlinePr summaryBelow="0" summaryRight="0"/>
-  </sheetPr>
-  <dimension ref="A1:D32"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="12.625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="3.75" customWidth="1"/>
-    <col min="2" max="2" width="30.5" customWidth="1"/>
-    <col min="3" max="3" width="30.125" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" s="27"/>
-      <c r="B1" s="27"/>
-      <c r="C1" s="27" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="28" t="s">
-        <v>110</v>
-      </c>
-      <c r="B2" s="28" t="s">
-        <v>111</v>
-      </c>
-      <c r="C2" s="28" t="s">
-        <v>112</v>
-      </c>
-      <c r="D2" s="28" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="29">
-        <v>1</v>
-      </c>
-      <c r="B3" s="30"/>
-      <c r="C3" s="30" t="s">
-        <v>114</v>
-      </c>
-      <c r="D3" s="30" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" s="29">
-        <v>1</v>
-      </c>
-      <c r="B4" s="30"/>
-      <c r="C4" s="30" t="s">
-        <v>116</v>
-      </c>
-      <c r="D4" s="30" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" s="29">
-        <v>5</v>
-      </c>
-      <c r="B5" s="30" t="s">
-        <v>118</v>
-      </c>
-      <c r="C5" s="30" t="s">
-        <v>119</v>
-      </c>
-      <c r="D5" s="30" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" s="29">
-        <v>1</v>
-      </c>
-      <c r="B6" s="30" t="s">
-        <v>121</v>
-      </c>
-      <c r="C6" s="30" t="s">
-        <v>122</v>
-      </c>
-      <c r="D6" s="30"/>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" s="29">
-        <v>1</v>
-      </c>
-      <c r="B7" s="30" t="s">
-        <v>123</v>
-      </c>
-      <c r="C7" s="30" t="s">
-        <v>124</v>
-      </c>
-      <c r="D7" s="30" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" s="29">
-        <v>4</v>
-      </c>
-      <c r="B8" s="30" t="s">
-        <v>126</v>
-      </c>
-      <c r="C8" s="30" t="s">
-        <v>127</v>
-      </c>
-      <c r="D8" s="30" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" s="29">
-        <v>1</v>
-      </c>
-      <c r="B9" s="30" t="s">
-        <v>129</v>
-      </c>
-      <c r="C9" s="30" t="s">
-        <v>130</v>
-      </c>
-      <c r="D9" s="30" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" s="29">
-        <v>1</v>
-      </c>
-      <c r="B10" s="30" t="s">
-        <v>131</v>
-      </c>
-      <c r="C10" s="30" t="s">
-        <v>132</v>
-      </c>
-      <c r="D10" s="30" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" s="29">
-        <v>1</v>
-      </c>
-      <c r="B11" s="30" t="s">
-        <v>134</v>
-      </c>
-      <c r="C11" s="30" t="s">
-        <v>135</v>
-      </c>
-      <c r="D11" s="30"/>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12" s="29">
-        <v>3</v>
-      </c>
-      <c r="B12" s="30" t="s">
-        <v>136</v>
-      </c>
-      <c r="C12" s="30" t="s">
-        <v>137</v>
-      </c>
-      <c r="D12" s="30" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A13" s="29">
-        <v>2</v>
-      </c>
-      <c r="B13" s="30" t="s">
-        <v>138</v>
-      </c>
-      <c r="C13" s="30" t="s">
-        <v>139</v>
-      </c>
-      <c r="D13" s="30" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A14" s="29">
-        <v>2</v>
-      </c>
-      <c r="B14" s="30" t="s">
-        <v>140</v>
-      </c>
-      <c r="C14" s="30" t="s">
-        <v>141</v>
-      </c>
-      <c r="D14" s="30" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A15" s="29">
-        <v>1</v>
-      </c>
-      <c r="B15" s="30" t="s">
-        <v>142</v>
-      </c>
-      <c r="C15" s="30" t="s">
-        <v>143</v>
-      </c>
-      <c r="D15" s="30" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A16" s="29">
-        <v>1</v>
-      </c>
-      <c r="B16" s="30" t="s">
-        <v>144</v>
-      </c>
-      <c r="C16" s="30" t="s">
-        <v>145</v>
-      </c>
-      <c r="D16" s="30" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17" s="29">
-        <v>1</v>
-      </c>
-      <c r="B17" s="30" t="s">
-        <v>146</v>
-      </c>
-      <c r="C17" s="30" t="s">
-        <v>147</v>
-      </c>
-      <c r="D17" s="30"/>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A18" s="29">
-        <v>1</v>
-      </c>
-      <c r="B18" s="30" t="s">
-        <v>148</v>
-      </c>
-      <c r="C18" s="30" t="s">
-        <v>149</v>
-      </c>
-      <c r="D18" s="30" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A19" s="29">
-        <v>1</v>
-      </c>
-      <c r="B19" s="30" t="s">
-        <v>151</v>
-      </c>
-      <c r="C19" s="30" t="s">
-        <v>152</v>
-      </c>
-      <c r="D19" s="30" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A20" s="29">
-        <v>1</v>
-      </c>
-      <c r="B20" s="30" t="s">
-        <v>154</v>
-      </c>
-      <c r="C20" s="30" t="s">
-        <v>155</v>
-      </c>
-      <c r="D20" s="30"/>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A21" s="29">
-        <v>1</v>
-      </c>
-      <c r="B21" s="30" t="s">
-        <v>156</v>
-      </c>
-      <c r="C21" s="30" t="s">
-        <v>157</v>
-      </c>
-      <c r="D21" s="27"/>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A22" s="29">
-        <v>1</v>
-      </c>
-      <c r="B22" s="30" t="s">
-        <v>158</v>
-      </c>
-      <c r="C22" s="30" t="s">
-        <v>159</v>
-      </c>
-      <c r="D22" s="30" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A23" s="29">
-        <v>1</v>
-      </c>
-      <c r="B23" s="30" t="s">
-        <v>161</v>
-      </c>
-      <c r="C23" s="30" t="s">
-        <v>162</v>
-      </c>
-      <c r="D23" s="30"/>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A24" s="29">
-        <v>2</v>
-      </c>
-      <c r="B24" s="30" t="s">
-        <v>163</v>
-      </c>
-      <c r="C24" s="30" t="s">
-        <v>164</v>
-      </c>
-      <c r="D24" s="30" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A25" s="29">
-        <v>1</v>
-      </c>
-      <c r="B25" s="30" t="s">
-        <v>166</v>
-      </c>
-      <c r="C25" s="30" t="s">
-        <v>167</v>
-      </c>
-      <c r="D25" s="30" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A26" s="29">
-        <v>1</v>
-      </c>
-      <c r="B26" s="30" t="s">
-        <v>168</v>
-      </c>
-      <c r="C26" s="30" t="s">
-        <v>169</v>
-      </c>
-      <c r="D26" s="30"/>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A27" s="29">
-        <v>1</v>
-      </c>
-      <c r="B27" s="30" t="s">
-        <v>170</v>
-      </c>
-      <c r="C27" s="30" t="s">
-        <v>171</v>
-      </c>
-      <c r="D27" s="30"/>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A28" s="29">
-        <v>2</v>
-      </c>
-      <c r="B28" s="30" t="s">
-        <v>172</v>
-      </c>
-      <c r="C28" s="37" t="s">
-        <v>173</v>
-      </c>
-      <c r="D28" s="38"/>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A29" s="29">
-        <v>1</v>
-      </c>
-      <c r="B29" s="30" t="s">
-        <v>174</v>
-      </c>
-      <c r="C29" s="30" t="s">
-        <v>175</v>
-      </c>
-      <c r="D29" s="30"/>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A30" s="29">
-        <v>1</v>
-      </c>
-      <c r="B30" s="30" t="s">
-        <v>176</v>
-      </c>
-      <c r="C30" s="30" t="s">
-        <v>177</v>
-      </c>
-      <c r="D30" s="27"/>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B32" s="31"/>
-    </row>
-  </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="C28:D28"/>
-  </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
Added TGM Production files
Added fab files for TGM's case, and updating MC1.1's PBS. TGM PBS is WIP.
</commit_message>
<xml_diff>
--- a/Medium Collar/MC1.1 Mk1 PBS.xlsx
+++ b/Medium Collar/MC1.1 Mk1 PBS.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24701"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24729"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Storage\Documents\GitHub\Trak-TFRC-System\Medium Collar\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F84CE32-8077-4941-9485-C7E8AD3ED817}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB1FA63C-0ECE-44D3-8D1F-CD372D7583D9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="PBS" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="109">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="113">
   <si>
     <t>Pricing</t>
   </si>
@@ -444,6 +444,18 @@
   <si>
     <t>MediumCollar1.1 Mk1 (Electronic Release)</t>
   </si>
+  <si>
+    <t>https://robokits.co.in/motor-drives-drivers/dc-motor-driver/two-way-motor-drive-module-drv8833</t>
+  </si>
+  <si>
+    <t>Motor Driver PCB</t>
+  </si>
+  <si>
+    <t>Robokits</t>
+  </si>
+  <si>
+    <t>MC1A01-015</t>
+  </si>
 </sst>
 </file>
 
@@ -452,7 +464,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="&quot;₹&quot;\ #,##0"/>
   </numFmts>
-  <fonts count="12" x14ac:knownFonts="1">
+  <fonts count="13" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -515,6 +527,10 @@
     <font>
       <sz val="10"/>
       <color rgb="FFFFC000"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Arial"/>
     </font>
   </fonts>
@@ -624,7 +640,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="34">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="164" fontId="1" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -669,6 +685,8 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -887,7 +905,7 @@
   <dimension ref="A1:P1000"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="M19" sqref="M19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1005,7 +1023,7 @@
       <c r="K3" s="13"/>
       <c r="L3" s="13">
         <f>SUM(L4:L36)</f>
-        <v>1336</v>
+        <v>1434</v>
       </c>
       <c r="M3" s="13">
         <f>SUM(M4:M21)</f>
@@ -1067,7 +1085,7 @@
         <v>360</v>
       </c>
       <c r="L5" s="13">
-        <f t="shared" ref="L5:L18" si="0">G5*K5</f>
+        <f t="shared" ref="L5:L19" si="0">G5*K5</f>
         <v>360</v>
       </c>
       <c r="M5" s="13"/>
@@ -1114,8 +1132,8 @@
       <c r="B7" s="16" t="s">
         <v>33</v>
       </c>
-      <c r="C7" s="17" t="s">
-        <v>25</v>
+      <c r="C7" s="33" t="s">
+        <v>99</v>
       </c>
       <c r="G7" s="16">
         <v>1</v>
@@ -1482,7 +1500,35 @@
         <v>18</v>
       </c>
     </row>
-    <row r="19" spans="1:16" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A19" s="8" t="s">
+        <v>112</v>
+      </c>
+      <c r="B19" s="32" t="s">
+        <v>110</v>
+      </c>
+      <c r="C19" s="33" t="s">
+        <v>99</v>
+      </c>
+      <c r="F19" t="s">
+        <v>111</v>
+      </c>
+      <c r="G19" s="32">
+        <v>1</v>
+      </c>
+      <c r="I19" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="J19" t="s">
+        <v>109</v>
+      </c>
+      <c r="K19">
+        <v>98</v>
+      </c>
+      <c r="L19" s="13">
+        <f t="shared" si="0"/>
+        <v>98</v>
+      </c>
       <c r="O19" s="14"/>
       <c r="P19" s="14" t="s">
         <v>83</v>
@@ -2648,8 +2694,9 @@
     <mergeCell ref="K1:L1"/>
     <mergeCell ref="O1:P1"/>
   </mergeCells>
-  <dataValidations count="3">
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="C5:C18" xr:uid="{00000000-0002-0000-0000-000000000000}">
+  <phoneticPr fontId="12" type="noConversion"/>
+  <dataValidations disablePrompts="1" count="3">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="C5:C19" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1>$P$26:$P$33</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="E5 E22" xr:uid="{00000000-0002-0000-0000-000001000000}">

</xml_diff>